<commit_message>
version 1 of the DD
</commit_message>
<xml_diff>
--- a/Effort/EffortMassimilianoBonettiDD.xlsx
+++ b/Effort/EffortMassimilianoBonettiDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/SE2proj/AbboAccordiBonetti/Effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA33C522-E604-B646-847A-0A09A75569CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346849DA-A2A8-E445-BEBC-4FC26B853BD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16440" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Massimiliano Bonetti</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Hours</t>
-  </si>
-  <si>
-    <t>Introduction</t>
   </si>
   <si>
     <t>Architectural Design</t>
@@ -420,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2283A0BD-A3F0-6040-B65F-FBDAEAD5CFA1}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +460,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -471,7 +468,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -479,7 +476,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -487,15 +484,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>